<commit_message>
add links to available images
</commit_message>
<xml_diff>
--- a/tests/dfi-dpi-change-check.xlsx
+++ b/tests/dfi-dpi-change-check.xlsx
@@ -1,11 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="25718"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="25601"/>
   <workbookPr defaultThemeVersion="166925"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{0FB8D525-1B54-4AB5-AD0B-E88647FA058A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\NZ\Documents\GitHub\dataframe_image_dpi\dataframe_image\tests\"/>
+    </mc:Choice>
+  </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8D0D3001-8E33-412A-A138-BBE0FF2A65C2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="105" windowWidth="14805" windowHeight="8010" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="29258" yWindow="765" windowWidth="17752" windowHeight="11535" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -16,12 +21,9 @@
     <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
       <xcalcf:calcFeatures>
         <xcalcf:feature name="microsoft.com:RD"/>
-        <xcalcf:feature name="microsoft.com:Single"/>
         <xcalcf:feature name="microsoft.com:FV"/>
-        <xcalcf:feature name="microsoft.com:CNMTM"/>
         <xcalcf:feature name="microsoft.com:LET_WF"/>
         <xcalcf:feature name="microsoft.com:LAMBDA_WF"/>
-        <xcalcf:feature name="microsoft.com:ARRAYTEXT_WF"/>
       </xcalcf:calcFeatures>
     </ext>
   </extLst>
@@ -29,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="33" uniqueCount="15">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="45" uniqueCount="20">
   <si>
     <t>Check</t>
   </si>
@@ -74,13 +76,28 @@
   </si>
   <si>
     <t>Y</t>
+  </si>
+  <si>
+    <t>test_output\covid19_mpl.png</t>
+  </si>
+  <si>
+    <t>test_output\covid19_mpl_dpi_600.png</t>
+  </si>
+  <si>
+    <t>test_output\covid19.png</t>
+  </si>
+  <si>
+    <t>test_output\covid19_styled.png</t>
+  </si>
+  <si>
+    <t>test_output\covid19_styled_dpi_400.png</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="2">
+  <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -92,6 +109,14 @@
       <b/>
       <sz val="11"/>
       <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color theme="10"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -123,7 +148,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="12">
+  <borders count="15">
     <border>
       <left/>
       <right/>
@@ -139,37 +164,6 @@
       <top style="medium">
         <color rgb="FF000000"/>
       </top>
-      <bottom/>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right style="medium">
-        <color rgb="FF000000"/>
-      </right>
-      <top style="medium">
-        <color rgb="FF000000"/>
-      </top>
-      <bottom/>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right style="medium">
-        <color rgb="FF000000"/>
-      </right>
-      <top/>
-      <bottom/>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="medium">
-        <color rgb="FF000000"/>
-      </left>
-      <right/>
-      <top style="medium">
-        <color rgb="FF000000"/>
-      </top>
       <bottom style="medium">
         <color rgb="FF000000"/>
       </bottom>
@@ -178,19 +172,6 @@
     <border>
       <left/>
       <right/>
-      <top style="medium">
-        <color rgb="FF000000"/>
-      </top>
-      <bottom style="medium">
-        <color rgb="FF000000"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right style="medium">
-        <color rgb="FF000000"/>
-      </right>
       <top style="medium">
         <color rgb="FF000000"/>
       </top>
@@ -209,8 +190,80 @@
       <diagonal/>
     </border>
     <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
       <left/>
       <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color rgb="FF000000"/>
+      </right>
+      <top style="medium">
+        <color rgb="FF000000"/>
+      </top>
+      <bottom style="medium">
+        <color rgb="FF000000"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top style="medium">
+        <color rgb="FF000000"/>
+      </top>
+      <bottom style="medium">
+        <color rgb="FF000000"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color rgb="FF000000"/>
+      </right>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
         <color rgb="FF000000"/>
       </right>
       <top/>
@@ -220,77 +273,92 @@
       <diagonal/>
     </border>
     <border>
+      <left/>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom style="thin">
+        <color rgb="FF000000"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
       <left style="medium">
-        <color rgb="FF000000"/>
+        <color indexed="64"/>
       </left>
       <right style="thin">
         <color rgb="FF000000"/>
       </right>
-      <top style="medium">
-        <color rgb="FF000000"/>
-      </top>
+      <top/>
       <bottom style="medium">
-        <color rgb="FF000000"/>
+        <color indexed="64"/>
       </bottom>
       <diagonal/>
     </border>
     <border>
+      <left/>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
       <left style="medium">
-        <color rgb="FF000000"/>
+        <color indexed="64"/>
       </left>
       <right style="thin">
-        <color rgb="FF000000"/>
+        <color indexed="64"/>
       </right>
       <top/>
       <bottom/>
       <diagonal/>
     </border>
-    <border>
-      <left style="medium">
-        <color rgb="FF000000"/>
-      </left>
-      <right style="thin">
-        <color rgb="FF000000"/>
-      </right>
-      <top/>
-      <bottom style="thin">
-        <color rgb="FF000000"/>
-      </bottom>
-      <diagonal/>
-    </border>
   </borders>
-  <cellStyleXfs count="1">
+  <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="22">
+  <cellXfs count="28">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="3" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="7" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="3" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="2" fontId="0" fillId="3" borderId="3" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="2" fontId="0" fillId="4" borderId="8" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="2" fontId="0" fillId="4" borderId="9" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="2" fontId="0" fillId="3" borderId="8" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="3" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="2" fontId="0" fillId="3" borderId="9" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="2" fontId="0" fillId="3" borderId="10" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="2" fontId="0" fillId="3" borderId="11" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="10" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="2" fontId="0" fillId="4" borderId="10" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="2" fontId="0" fillId="4" borderId="3" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="8" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="9" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="2" fontId="0" fillId="3" borderId="12" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="2" fontId="0" fillId="3" borderId="13" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="2" fontId="0" fillId="3" borderId="14" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="1"/>
   </cellXfs>
-  <cellStyles count="1">
+  <cellStyles count="2">
+    <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -652,234 +720,250 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A2:H11"/>
+  <dimension ref="A1:I13"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="H4" sqref="A4:H4"/>
+      <selection activeCell="E22" sqref="E22"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
   <cols>
-    <col min="2" max="2" width="16.5703125" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="7.42578125" customWidth="1"/>
-    <col min="4" max="4" width="11.7109375" customWidth="1"/>
+    <col min="2" max="2" width="16.59765625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="7.3984375" customWidth="1"/>
+    <col min="4" max="4" width="11.73046875" customWidth="1"/>
     <col min="5" max="5" width="8" customWidth="1"/>
     <col min="6" max="6" width="9" customWidth="1"/>
-    <col min="7" max="7" width="25.140625" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="25.1328125" bestFit="1" customWidth="1"/>
     <col min="8" max="8" width="26" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="1:8">
-      <c r="G2" s="2" t="s">
+    <row r="1" spans="1:9" ht="14.65" thickBot="1" x14ac:dyDescent="0.5"/>
+    <row r="2" spans="1:9" ht="14.65" thickBot="1" x14ac:dyDescent="0.5">
+      <c r="G2" s="12" t="s">
         <v>0</v>
       </c>
-      <c r="H2" s="3"/>
-    </row>
-    <row r="3" spans="1:8" s="1" customFormat="1">
-      <c r="A3" s="4" t="s">
+      <c r="H2" s="13"/>
+    </row>
+    <row r="3" spans="1:9" s="1" customFormat="1" ht="14.65" thickBot="1" x14ac:dyDescent="0.5">
+      <c r="A3" s="2" t="s">
         <v>1</v>
       </c>
-      <c r="B3" s="5" t="s">
+      <c r="B3" s="3" t="s">
         <v>2</v>
       </c>
-      <c r="C3" s="5" t="s">
+      <c r="C3" s="3" t="s">
         <v>3</v>
       </c>
-      <c r="D3" s="6" t="s">
+      <c r="D3" s="4" t="s">
         <v>4</v>
       </c>
-      <c r="E3" s="5" t="s">
+      <c r="E3" s="3" t="s">
         <v>5</v>
       </c>
-      <c r="F3" s="5" t="s">
+      <c r="F3" s="3" t="s">
         <v>6</v>
       </c>
-      <c r="G3" s="15" t="s">
+      <c r="G3" s="14" t="s">
         <v>7</v>
       </c>
-      <c r="H3" s="11" t="s">
+      <c r="H3" s="15" t="s">
         <v>8</v>
       </c>
     </row>
-    <row r="4" spans="1:8">
-      <c r="A4" s="19" t="s">
+    <row r="4" spans="1:9" x14ac:dyDescent="0.45">
+      <c r="A4" s="8" t="s">
         <v>9</v>
       </c>
-      <c r="B4" s="19" t="s">
+      <c r="B4" s="8" t="s">
         <v>10</v>
       </c>
-      <c r="C4" s="19" t="s">
+      <c r="C4" s="8" t="s">
         <v>11</v>
       </c>
-      <c r="D4" s="19">
+      <c r="D4" s="8">
         <v>100</v>
       </c>
-      <c r="E4" s="19">
+      <c r="E4" s="8">
         <v>696</v>
       </c>
-      <c r="F4" s="19">
+      <c r="F4" s="8">
         <v>466</v>
       </c>
-      <c r="G4" s="20"/>
-      <c r="H4" s="21"/>
-    </row>
-    <row r="5" spans="1:8">
-      <c r="A5" s="7" t="s">
+      <c r="G4" s="16"/>
+      <c r="H4" s="17"/>
+      <c r="I4" s="27" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="5" spans="1:9" x14ac:dyDescent="0.45">
+      <c r="A5" t="s">
         <v>12</v>
       </c>
-      <c r="B5" s="7" t="s">
+      <c r="B5" t="s">
         <v>10</v>
       </c>
-      <c r="C5" s="7" t="s">
+      <c r="C5" t="s">
         <v>11</v>
       </c>
-      <c r="D5" s="8">
+      <c r="D5" s="5">
         <v>400</v>
       </c>
-      <c r="E5" s="7">
+      <c r="E5">
         <v>2786</v>
       </c>
-      <c r="F5" s="7">
+      <c r="F5">
         <v>1866</v>
       </c>
-      <c r="G5" s="16">
+      <c r="G5" s="18">
         <f>E5/E4</f>
         <v>4.0028735632183912</v>
       </c>
-      <c r="H5" s="12">
+      <c r="H5" s="19">
         <f>F5/F4</f>
         <v>4.0042918454935625</v>
       </c>
     </row>
-    <row r="6" spans="1:8">
-      <c r="A6" s="9" t="s">
+    <row r="6" spans="1:9" x14ac:dyDescent="0.45">
+      <c r="A6" s="6" t="s">
         <v>12</v>
       </c>
-      <c r="B6" s="9" t="s">
+      <c r="B6" s="6" t="s">
         <v>10</v>
       </c>
-      <c r="C6" s="9" t="s">
+      <c r="C6" s="6" t="s">
         <v>11</v>
       </c>
-      <c r="D6" s="10">
+      <c r="D6" s="7">
         <v>600</v>
       </c>
-      <c r="E6" s="9">
+      <c r="E6" s="6">
         <v>4179</v>
       </c>
-      <c r="F6" s="9">
+      <c r="F6" s="6">
         <v>2800</v>
       </c>
-      <c r="G6" s="17">
+      <c r="G6" s="20">
         <f>E6/E4</f>
         <v>6.0043103448275863</v>
       </c>
-      <c r="H6" s="13">
+      <c r="H6" s="21">
         <f>F6/F4</f>
         <v>6.0085836909871242</v>
       </c>
-    </row>
-    <row r="7" spans="1:8">
-      <c r="A7" s="19" t="s">
+      <c r="I6" s="27" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="7" spans="1:9" x14ac:dyDescent="0.45">
+      <c r="A7" s="8" t="s">
         <v>9</v>
       </c>
-      <c r="B7" s="19" t="s">
+      <c r="B7" s="8" t="s">
         <v>13</v>
       </c>
-      <c r="C7" s="19" t="s">
+      <c r="C7" s="8" t="s">
         <v>11</v>
       </c>
-      <c r="D7" s="19">
+      <c r="D7" s="8">
         <v>100</v>
       </c>
-      <c r="E7" s="19">
+      <c r="E7" s="8">
         <v>462</v>
       </c>
-      <c r="F7" s="19">
+      <c r="F7" s="8">
         <v>356</v>
       </c>
-      <c r="G7" s="20"/>
-      <c r="H7" s="21"/>
-    </row>
-    <row r="8" spans="1:8">
-      <c r="A8" s="7" t="s">
+      <c r="G7" s="16"/>
+      <c r="H7" s="17"/>
+      <c r="I7" s="27" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="8" spans="1:9" x14ac:dyDescent="0.45">
+      <c r="A8" t="s">
         <v>12</v>
       </c>
-      <c r="B8" s="7" t="s">
+      <c r="B8" t="s">
         <v>13</v>
       </c>
-      <c r="C8" s="7" t="s">
+      <c r="C8" t="s">
         <v>11</v>
       </c>
-      <c r="D8" s="8">
+      <c r="D8" s="5">
         <v>400</v>
       </c>
-      <c r="E8" s="7">
+      <c r="E8">
         <v>1840</v>
       </c>
-      <c r="F8" s="7">
+      <c r="F8">
         <v>1424</v>
       </c>
-      <c r="G8" s="16">
+      <c r="G8" s="18">
         <f>E8/E7</f>
         <v>3.9826839826839828</v>
       </c>
-      <c r="H8" s="12">
+      <c r="H8" s="19">
         <f>F8/F7</f>
         <v>4</v>
       </c>
     </row>
-    <row r="9" spans="1:8">
-      <c r="A9" s="9" t="s">
+    <row r="9" spans="1:9" x14ac:dyDescent="0.45">
+      <c r="A9" s="6" t="s">
         <v>12</v>
       </c>
-      <c r="B9" s="9" t="s">
+      <c r="B9" s="6" t="s">
         <v>13</v>
       </c>
-      <c r="C9" s="9" t="s">
+      <c r="C9" s="6" t="s">
         <v>11</v>
       </c>
-      <c r="D9" s="10">
+      <c r="D9" s="7">
         <v>600</v>
       </c>
-      <c r="E9" s="9">
+      <c r="E9" s="6">
         <v>2760</v>
       </c>
-      <c r="F9" s="9">
+      <c r="F9" s="6">
         <v>2118</v>
       </c>
-      <c r="G9" s="17">
+      <c r="G9" s="20">
         <f>E9/E7</f>
         <v>5.9740259740259738</v>
       </c>
-      <c r="H9" s="13">
+      <c r="H9" s="21">
         <f>F9/F7</f>
         <v>5.9494382022471912</v>
       </c>
-    </row>
-    <row r="10" spans="1:8">
-      <c r="A10" s="7" t="s">
+      <c r="I9" s="27" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="10" spans="1:9" x14ac:dyDescent="0.45">
+      <c r="A10" t="s">
         <v>9</v>
       </c>
-      <c r="B10" s="7" t="s">
+      <c r="B10" t="s">
         <v>13</v>
       </c>
-      <c r="C10" s="7" t="s">
+      <c r="C10" t="s">
         <v>14</v>
       </c>
-      <c r="D10" s="8">
+      <c r="D10" s="5">
         <v>1</v>
       </c>
-      <c r="E10" s="7">
+      <c r="E10">
         <v>754</v>
       </c>
-      <c r="F10" s="7">
+      <c r="F10">
         <v>365</v>
       </c>
-      <c r="G10" s="18"/>
-      <c r="H10" s="14"/>
-    </row>
-    <row r="11" spans="1:8">
+      <c r="G10" s="22"/>
+      <c r="H10" s="23"/>
+      <c r="I10" s="27" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="11" spans="1:9" s="9" customFormat="1" x14ac:dyDescent="0.45">
       <c r="A11" s="9" t="s">
         <v>12</v>
       </c>
@@ -898,19 +982,70 @@
       <c r="F11" s="9">
         <v>1464</v>
       </c>
-      <c r="G11" s="17">
-        <f>E11/E10</f>
-        <v>3.989389920424403</v>
-      </c>
-      <c r="H11" s="13">
-        <f>F11/F10</f>
-        <v>4.0109589041095894</v>
+      <c r="G11" s="26">
+        <f>E11/E8</f>
+        <v>1.6347826086956523</v>
+      </c>
+      <c r="H11" s="19">
+        <f>F11/F8</f>
+        <v>1.0280898876404494</v>
+      </c>
+    </row>
+    <row r="12" spans="1:9" x14ac:dyDescent="0.45">
+      <c r="A12" s="11" t="s">
+        <v>12</v>
+      </c>
+      <c r="B12" s="11" t="s">
+        <v>13</v>
+      </c>
+      <c r="C12" s="11" t="s">
+        <v>14</v>
+      </c>
+      <c r="D12" s="5">
+        <v>400</v>
+      </c>
+      <c r="G12" s="22"/>
+      <c r="H12" s="23"/>
+      <c r="I12" s="27" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="13" spans="1:9" ht="14.65" thickBot="1" x14ac:dyDescent="0.5">
+      <c r="A13" s="6" t="s">
+        <v>12</v>
+      </c>
+      <c r="B13" s="6" t="s">
+        <v>13</v>
+      </c>
+      <c r="C13" s="6" t="s">
+        <v>14</v>
+      </c>
+      <c r="D13" s="7">
+        <v>600</v>
+      </c>
+      <c r="E13" s="6"/>
+      <c r="F13" s="6"/>
+      <c r="G13" s="24">
+        <f>E13/E10</f>
+        <v>0</v>
+      </c>
+      <c r="H13" s="25">
+        <f>F13/F10</f>
+        <v>0</v>
       </c>
     </row>
   </sheetData>
   <mergeCells count="1">
     <mergeCell ref="G2:H2"/>
   </mergeCells>
+  <hyperlinks>
+    <hyperlink ref="I4" r:id="rId1" xr:uid="{38E1FA5E-B128-4BDB-81C3-0DF1F3E0A50F}"/>
+    <hyperlink ref="I6" r:id="rId2" xr:uid="{BEDC4C2C-B763-42AB-810F-DDD115D81A3F}"/>
+    <hyperlink ref="I7" r:id="rId3" xr:uid="{3AEC8C0D-8F29-42B4-B143-754EED71C400}"/>
+    <hyperlink ref="I9" r:id="rId4" xr:uid="{4C56F69D-D263-4563-91DB-EB4489269245}"/>
+    <hyperlink ref="I10" r:id="rId5" xr:uid="{69B48664-D1A6-410B-9FE5-12E8D566C68E}"/>
+    <hyperlink ref="I12" r:id="rId6" xr:uid="{A9574FF3-3FBB-4407-8533-14361E98328D}"/>
+  </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
@@ -923,7 +1058,7 @@
       <selection activeCell="I11" sqref="I11"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
   <sheetData/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <drawing r:id="rId1"/>

</xml_diff>

<commit_message>
[WIP] test out changes to dpi/scale factor
</commit_message>
<xml_diff>
--- a/tests/dfi-dpi-change-check.xlsx
+++ b/tests/dfi-dpi-change-check.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\NZ\Documents\GitHub\dataframe_image_dpi\dataframe_image\tests\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8D0D3001-8E33-412A-A138-BBE0FF2A65C2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{551CE241-3562-45DC-8D80-D6B60F3B6901}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="29258" yWindow="765" windowWidth="17752" windowHeight="11535" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -31,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="45" uniqueCount="20">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="46" uniqueCount="21">
   <si>
     <t>Check</t>
   </si>
@@ -91,13 +91,16 @@
   </si>
   <si>
     <t>test_output\covid19_styled_dpi_400.png</t>
+  </si>
+  <si>
+    <t>Ensure tests have run successfully (for links to work)</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="3" x14ac:knownFonts="1">
+  <fonts count="4" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -117,6 +120,14 @@
       <u/>
       <sz val="11"/>
       <color theme="10"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <i/>
+      <sz val="11"/>
+      <color theme="1"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -323,7 +334,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="28">
+  <cellXfs count="26">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
@@ -333,15 +344,6 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="3" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="1" fillId="3" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="3" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="2" fontId="0" fillId="4" borderId="8" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
@@ -356,6 +358,13 @@
     <xf numFmtId="2" fontId="0" fillId="3" borderId="13" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="2" fontId="0" fillId="3" borderId="14" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
@@ -723,7 +732,7 @@
   <dimension ref="A1:I13"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E22" sqref="E22"/>
+      <selection activeCell="I8" sqref="I8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
@@ -739,10 +748,10 @@
   <sheetData>
     <row r="1" spans="1:9" ht="14.65" thickBot="1" x14ac:dyDescent="0.5"/>
     <row r="2" spans="1:9" ht="14.65" thickBot="1" x14ac:dyDescent="0.5">
-      <c r="G2" s="12" t="s">
+      <c r="G2" s="23" t="s">
         <v>0</v>
       </c>
-      <c r="H2" s="13"/>
+      <c r="H2" s="24"/>
     </row>
     <row r="3" spans="1:9" s="1" customFormat="1" ht="14.65" thickBot="1" x14ac:dyDescent="0.5">
       <c r="A3" s="2" t="s">
@@ -763,11 +772,14 @@
       <c r="F3" s="3" t="s">
         <v>6</v>
       </c>
-      <c r="G3" s="14" t="s">
+      <c r="G3" s="9" t="s">
         <v>7</v>
       </c>
-      <c r="H3" s="15" t="s">
+      <c r="H3" s="10" t="s">
         <v>8</v>
+      </c>
+      <c r="I3" s="25" t="s">
+        <v>20</v>
       </c>
     </row>
     <row r="4" spans="1:9" x14ac:dyDescent="0.45">
@@ -789,9 +801,9 @@
       <c r="F4" s="8">
         <v>466</v>
       </c>
-      <c r="G4" s="16"/>
-      <c r="H4" s="17"/>
-      <c r="I4" s="27" t="s">
+      <c r="G4" s="11"/>
+      <c r="H4" s="12"/>
+      <c r="I4" s="22" t="s">
         <v>15</v>
       </c>
     </row>
@@ -814,11 +826,11 @@
       <c r="F5">
         <v>1866</v>
       </c>
-      <c r="G5" s="18">
+      <c r="G5" s="13">
         <f>E5/E4</f>
         <v>4.0028735632183912</v>
       </c>
-      <c r="H5" s="19">
+      <c r="H5" s="14">
         <f>F5/F4</f>
         <v>4.0042918454935625</v>
       </c>
@@ -842,15 +854,15 @@
       <c r="F6" s="6">
         <v>2800</v>
       </c>
-      <c r="G6" s="20">
+      <c r="G6" s="15">
         <f>E6/E4</f>
         <v>6.0043103448275863</v>
       </c>
-      <c r="H6" s="21">
+      <c r="H6" s="16">
         <f>F6/F4</f>
         <v>6.0085836909871242</v>
       </c>
-      <c r="I6" s="27" t="s">
+      <c r="I6" s="22" t="s">
         <v>16</v>
       </c>
     </row>
@@ -873,9 +885,9 @@
       <c r="F7" s="8">
         <v>356</v>
       </c>
-      <c r="G7" s="16"/>
-      <c r="H7" s="17"/>
-      <c r="I7" s="27" t="s">
+      <c r="G7" s="11"/>
+      <c r="H7" s="12"/>
+      <c r="I7" s="22" t="s">
         <v>17</v>
       </c>
     </row>
@@ -898,11 +910,11 @@
       <c r="F8">
         <v>1424</v>
       </c>
-      <c r="G8" s="18">
+      <c r="G8" s="13">
         <f>E8/E7</f>
         <v>3.9826839826839828</v>
       </c>
-      <c r="H8" s="19">
+      <c r="H8" s="14">
         <f>F8/F7</f>
         <v>4</v>
       </c>
@@ -926,15 +938,15 @@
       <c r="F9" s="6">
         <v>2118</v>
       </c>
-      <c r="G9" s="20">
+      <c r="G9" s="15">
         <f>E9/E7</f>
         <v>5.9740259740259738</v>
       </c>
-      <c r="H9" s="21">
+      <c r="H9" s="16">
         <f>F9/F7</f>
         <v>5.9494382022471912</v>
       </c>
-      <c r="I9" s="27" t="s">
+      <c r="I9" s="22" t="s">
         <v>16</v>
       </c>
     </row>
@@ -957,56 +969,56 @@
       <c r="F10">
         <v>365</v>
       </c>
-      <c r="G10" s="22"/>
-      <c r="H10" s="23"/>
-      <c r="I10" s="27" t="s">
+      <c r="G10" s="17"/>
+      <c r="H10" s="18"/>
+      <c r="I10" s="22" t="s">
         <v>18</v>
       </c>
     </row>
-    <row r="11" spans="1:9" s="9" customFormat="1" x14ac:dyDescent="0.45">
-      <c r="A11" s="9" t="s">
+    <row r="11" spans="1:9" x14ac:dyDescent="0.45">
+      <c r="A11" t="s">
         <v>12</v>
       </c>
-      <c r="B11" s="9" t="s">
+      <c r="B11" t="s">
         <v>13</v>
       </c>
-      <c r="C11" s="9" t="s">
+      <c r="C11" t="s">
         <v>14</v>
       </c>
-      <c r="D11" s="10">
+      <c r="D11" s="5">
         <v>4</v>
       </c>
-      <c r="E11" s="9">
+      <c r="E11">
         <v>3008</v>
       </c>
-      <c r="F11" s="9">
+      <c r="F11">
         <v>1464</v>
       </c>
-      <c r="G11" s="26">
+      <c r="G11" s="21">
         <f>E11/E8</f>
         <v>1.6347826086956523</v>
       </c>
-      <c r="H11" s="19">
+      <c r="H11" s="14">
         <f>F11/F8</f>
         <v>1.0280898876404494</v>
       </c>
     </row>
     <row r="12" spans="1:9" x14ac:dyDescent="0.45">
-      <c r="A12" s="11" t="s">
+      <c r="A12" t="s">
         <v>12</v>
       </c>
-      <c r="B12" s="11" t="s">
+      <c r="B12" t="s">
         <v>13</v>
       </c>
-      <c r="C12" s="11" t="s">
+      <c r="C12" t="s">
         <v>14</v>
       </c>
       <c r="D12" s="5">
         <v>400</v>
       </c>
-      <c r="G12" s="22"/>
-      <c r="H12" s="23"/>
-      <c r="I12" s="27" t="s">
+      <c r="G12" s="17"/>
+      <c r="H12" s="18"/>
+      <c r="I12" s="22" t="s">
         <v>19</v>
       </c>
     </row>
@@ -1025,11 +1037,11 @@
       </c>
       <c r="E13" s="6"/>
       <c r="F13" s="6"/>
-      <c r="G13" s="24">
+      <c r="G13" s="19">
         <f>E13/E10</f>
         <v>0</v>
       </c>
-      <c r="H13" s="25">
+      <c r="H13" s="20">
         <f>F13/F10</f>
         <v>0</v>
       </c>
@@ -1047,6 +1059,7 @@
     <hyperlink ref="I12" r:id="rId6" xr:uid="{A9574FF3-3FBB-4407-8533-14361E98328D}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId7"/>
 </worksheet>
 </file>
 

</xml_diff>

<commit_message>
had wrong height for default styled chrome export
</commit_message>
<xml_diff>
--- a/tests/dfi-dpi-change-check.xlsx
+++ b/tests/dfi-dpi-change-check.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\NZ\Documents\GitHub\dataframe_image_dpi\dataframe_image\tests\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{406ABA31-ED48-4EFF-9145-BA4F913DBC5E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{99FDAAA4-E2AE-4E12-918E-1AFF5C0C7228}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="35812" yWindow="1312" windowWidth="20768" windowHeight="11536" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -937,7 +937,7 @@
   <dimension ref="A1:I18"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D20" sqref="D20"/>
+      <selection activeCell="I15" sqref="I15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
@@ -1311,7 +1311,7 @@
       </c>
       <c r="H14" s="50">
         <f>F14/$F$15</f>
-        <v>0.45753424657534247</v>
+        <v>0.47308781869688388</v>
       </c>
       <c r="I14" s="34" t="s">
         <v>28</v>
@@ -1334,7 +1334,7 @@
         <v>754</v>
       </c>
       <c r="F15" s="18">
-        <v>365</v>
+        <v>353</v>
       </c>
       <c r="G15" s="16"/>
       <c r="H15" s="17"/>
@@ -1367,7 +1367,7 @@
       </c>
       <c r="H16" s="23">
         <f>F16/$F$15</f>
-        <v>3.8876712328767122</v>
+        <v>4.0198300283286121</v>
       </c>
       <c r="I16" s="34" t="s">
         <v>18</v>
@@ -1398,7 +1398,7 @@
       </c>
       <c r="H17" s="23">
         <f t="shared" ref="H17:H18" si="5">F17/$F$15</f>
-        <v>5.8136986301369866</v>
+        <v>6.0113314447592066</v>
       </c>
       <c r="I17" s="34" t="s">
         <v>30</v>
@@ -1429,7 +1429,7 @@
       </c>
       <c r="H18" s="25">
         <f t="shared" si="5"/>
-        <v>7.7369863013698632</v>
+        <v>8</v>
       </c>
       <c r="I18" s="36" t="s">
         <v>29</v>

</xml_diff>

<commit_message>
tweak default row fill color for DPI col
</commit_message>
<xml_diff>
--- a/tests/dfi-dpi-change-check.xlsx
+++ b/tests/dfi-dpi-change-check.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\NZ\Documents\GitHub\dataframe_image_dpi\dataframe_image\tests\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{99FDAAA4-E2AE-4E12-918E-1AFF5C0C7228}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A629A29B-5EAC-4D29-ACDB-437E4AA31276}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="35812" yWindow="1312" windowWidth="20768" windowHeight="11536" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -166,7 +166,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="6">
+  <fills count="5">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -176,12 +176,6 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor rgb="FFDDEBF7"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFF2CC"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -511,12 +505,9 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="54">
+  <cellXfs count="52">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1"/>
-    <xf numFmtId="2" fontId="0" fillId="3" borderId="3" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="2" fontId="0" fillId="3" borderId="4" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="2" fontId="0" fillId="2" borderId="3" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="2" fontId="0" fillId="2" borderId="4" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="2" fontId="0" fillId="2" borderId="5" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
@@ -532,13 +523,14 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="3" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="4" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="3" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="4" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="1"/>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="6" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="6" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="2" fontId="0" fillId="2" borderId="7" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="2" fontId="0" fillId="2" borderId="8" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="2" fontId="0" fillId="2" borderId="9" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
@@ -547,29 +539,29 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="12" xfId="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="1" fillId="5" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="4" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="16" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="17" xfId="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="17" xfId="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="18" xfId="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="16" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="2" fontId="0" fillId="3" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="19" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="20" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="20" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="20" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="2" fontId="0" fillId="2" borderId="21" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="22" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="22" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="22" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="23" xfId="0" applyBorder="1"/>
     <xf numFmtId="2" fontId="0" fillId="2" borderId="24" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="22" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="2" fontId="0" fillId="2" borderId="25" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="2" fontId="0" fillId="2" borderId="26" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="2" fontId="0" fillId="2" borderId="20" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="2" fontId="0" fillId="2" borderId="6" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="10" xfId="1" applyBorder="1"/>
+    <xf numFmtId="2" fontId="0" fillId="3" borderId="3" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="2" fontId="0" fillId="3" borderId="4" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="2" fontId="0" fillId="3" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
@@ -937,7 +929,7 @@
   <dimension ref="A1:I18"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="I15" sqref="I15"/>
+      <selection activeCell="C25" sqref="C25"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
@@ -954,93 +946,93 @@
   <sheetData>
     <row r="1" spans="1:9" ht="14.65" thickBot="1" x14ac:dyDescent="0.5"/>
     <row r="2" spans="1:9" ht="14.65" thickBot="1" x14ac:dyDescent="0.5">
-      <c r="G2" s="8" t="s">
+      <c r="G2" s="5" t="s">
         <v>0</v>
       </c>
-      <c r="H2" s="9"/>
+      <c r="H2" s="6"/>
     </row>
     <row r="3" spans="1:9" s="1" customFormat="1" ht="14.65" thickBot="1" x14ac:dyDescent="0.5">
-      <c r="A3" s="29" t="s">
+      <c r="A3" s="27" t="s">
         <v>1</v>
       </c>
-      <c r="B3" s="30" t="s">
+      <c r="B3" s="28" t="s">
         <v>2</v>
       </c>
-      <c r="C3" s="30" t="s">
+      <c r="C3" s="28" t="s">
         <v>3</v>
       </c>
-      <c r="D3" s="31" t="s">
+      <c r="D3" s="29" t="s">
         <v>27</v>
       </c>
-      <c r="E3" s="30" t="s">
+      <c r="E3" s="28" t="s">
         <v>4</v>
       </c>
-      <c r="F3" s="30" t="s">
+      <c r="F3" s="28" t="s">
         <v>5</v>
       </c>
-      <c r="G3" s="32" t="s">
+      <c r="G3" s="30" t="s">
         <v>6</v>
       </c>
-      <c r="H3" s="37" t="s">
+      <c r="H3" s="35" t="s">
         <v>7</v>
       </c>
-      <c r="I3" s="33" t="s">
+      <c r="I3" s="31" t="s">
         <v>31</v>
       </c>
     </row>
-    <row r="4" spans="1:9" s="15" customFormat="1" x14ac:dyDescent="0.45">
-      <c r="A4" s="14" t="s">
+    <row r="4" spans="1:9" s="12" customFormat="1" x14ac:dyDescent="0.45">
+      <c r="A4" s="11" t="s">
         <v>25</v>
       </c>
-      <c r="B4" s="14" t="s">
+      <c r="B4" s="11" t="s">
         <v>9</v>
       </c>
-      <c r="C4" s="14" t="s">
+      <c r="C4" s="11" t="s">
         <v>10</v>
       </c>
-      <c r="D4" s="19">
+      <c r="D4" s="17">
         <v>50</v>
       </c>
-      <c r="E4" s="14">
+      <c r="E4" s="11">
         <v>348</v>
       </c>
-      <c r="F4" s="14">
+      <c r="F4" s="11">
         <v>233</v>
       </c>
-      <c r="G4" s="5">
+      <c r="G4" s="2">
         <f>E4/$E$5</f>
         <v>0.5</v>
       </c>
-      <c r="H4" s="6">
+      <c r="H4" s="3">
         <f>F4/$F$5</f>
         <v>0.5</v>
       </c>
-      <c r="I4" s="34" t="s">
+      <c r="I4" s="32" t="s">
         <v>26</v>
       </c>
     </row>
     <row r="5" spans="1:9" x14ac:dyDescent="0.45">
-      <c r="A5" s="2" t="s">
+      <c r="A5" s="13" t="s">
         <v>8</v>
       </c>
-      <c r="B5" s="2" t="s">
+      <c r="B5" s="13" t="s">
         <v>9</v>
       </c>
-      <c r="C5" s="2" t="s">
+      <c r="C5" s="13" t="s">
         <v>10</v>
       </c>
-      <c r="D5" s="20">
+      <c r="D5" s="13">
         <v>100</v>
       </c>
-      <c r="E5" s="2">
+      <c r="E5" s="13">
         <v>696</v>
       </c>
-      <c r="F5" s="2">
+      <c r="F5" s="13">
         <v>466</v>
       </c>
-      <c r="G5" s="3"/>
-      <c r="H5" s="4"/>
-      <c r="I5" s="34" t="s">
+      <c r="G5" s="49"/>
+      <c r="H5" s="50"/>
+      <c r="I5" s="32" t="s">
         <v>14</v>
       </c>
     </row>
@@ -1054,7 +1046,7 @@
       <c r="C6" t="s">
         <v>10</v>
       </c>
-      <c r="D6" s="20">
+      <c r="D6" s="18">
         <v>400</v>
       </c>
       <c r="E6">
@@ -1063,375 +1055,375 @@
       <c r="F6">
         <v>1866</v>
       </c>
-      <c r="G6" s="5">
+      <c r="G6" s="2">
         <f>E6/$E$5</f>
         <v>4.0028735632183912</v>
       </c>
-      <c r="H6" s="6">
+      <c r="H6" s="3">
         <f>F6/$F$5</f>
         <v>4.0042918454935625</v>
       </c>
-      <c r="I6" s="34" t="s">
+      <c r="I6" s="32" t="s">
         <v>19</v>
       </c>
     </row>
     <row r="7" spans="1:9" x14ac:dyDescent="0.45">
-      <c r="A7" s="11" t="s">
+      <c r="A7" s="8" t="s">
         <v>11</v>
       </c>
-      <c r="B7" s="11" t="s">
+      <c r="B7" s="8" t="s">
         <v>9</v>
       </c>
-      <c r="C7" s="11" t="s">
+      <c r="C7" s="8" t="s">
         <v>10</v>
       </c>
-      <c r="D7" s="21">
+      <c r="D7" s="19">
         <v>600</v>
       </c>
-      <c r="E7" s="11">
+      <c r="E7" s="8">
         <v>4179</v>
       </c>
-      <c r="F7" s="11">
+      <c r="F7" s="8">
         <v>2800</v>
       </c>
-      <c r="G7" s="5">
+      <c r="G7" s="2">
         <f t="shared" ref="G7:G8" si="0">E7/$E$5</f>
         <v>6.0043103448275863</v>
       </c>
-      <c r="H7" s="6">
+      <c r="H7" s="3">
         <f t="shared" ref="H7:H8" si="1">F7/$F$5</f>
         <v>6.0085836909871242</v>
       </c>
-      <c r="I7" s="34" t="s">
+      <c r="I7" s="32" t="s">
         <v>15</v>
       </c>
     </row>
     <row r="8" spans="1:9" x14ac:dyDescent="0.45">
-      <c r="A8" s="11" t="s">
+      <c r="A8" s="8" t="s">
         <v>11</v>
       </c>
-      <c r="B8" s="11" t="s">
+      <c r="B8" s="8" t="s">
         <v>9</v>
       </c>
-      <c r="C8" s="11" t="s">
+      <c r="C8" s="8" t="s">
         <v>10</v>
       </c>
-      <c r="D8" s="21">
+      <c r="D8" s="19">
         <v>800</v>
       </c>
-      <c r="E8" s="10">
+      <c r="E8" s="7">
         <v>5572</v>
       </c>
-      <c r="F8" s="10">
+      <c r="F8" s="7">
         <v>3733</v>
       </c>
-      <c r="G8" s="5">
+      <c r="G8" s="2">
         <f t="shared" si="0"/>
         <v>8.0057471264367823</v>
       </c>
-      <c r="H8" s="6">
+      <c r="H8" s="3">
         <f t="shared" si="1"/>
         <v>8.0107296137339059</v>
       </c>
-      <c r="I8" s="35" t="s">
+      <c r="I8" s="33" t="s">
         <v>23</v>
       </c>
     </row>
     <row r="9" spans="1:9" x14ac:dyDescent="0.45">
-      <c r="A9" s="39" t="s">
+      <c r="A9" s="36" t="s">
         <v>25</v>
       </c>
-      <c r="B9" s="40" t="s">
+      <c r="B9" s="37" t="s">
         <v>12</v>
       </c>
-      <c r="C9" s="40" t="s">
+      <c r="C9" s="37" t="s">
         <v>10</v>
       </c>
-      <c r="D9" s="41">
+      <c r="D9" s="38">
         <v>50</v>
       </c>
-      <c r="E9" s="40">
+      <c r="E9" s="37">
         <v>230</v>
       </c>
-      <c r="F9" s="40">
+      <c r="F9" s="37">
         <v>163</v>
       </c>
-      <c r="G9" s="46">
+      <c r="G9" s="43">
         <f>E9/$E$10</f>
         <v>0.5</v>
       </c>
-      <c r="H9" s="51">
+      <c r="H9" s="46">
         <f>F9/$F$10</f>
         <v>0.47521865889212828</v>
       </c>
-      <c r="I9" s="53" t="s">
+      <c r="I9" s="48" t="s">
         <v>24</v>
       </c>
     </row>
     <row r="10" spans="1:9" x14ac:dyDescent="0.45">
-      <c r="A10" s="47" t="s">
+      <c r="A10" s="40" t="s">
         <v>8</v>
       </c>
-      <c r="B10" s="48" t="s">
+      <c r="B10" s="16" t="s">
         <v>12</v>
       </c>
-      <c r="C10" s="48" t="s">
+      <c r="C10" s="16" t="s">
         <v>10</v>
       </c>
-      <c r="D10" s="21">
+      <c r="D10" s="16">
         <v>100</v>
       </c>
-      <c r="E10" s="48">
+      <c r="E10" s="16">
         <v>460</v>
       </c>
-      <c r="F10" s="48">
+      <c r="F10" s="16">
         <v>343</v>
       </c>
-      <c r="G10" s="3"/>
-      <c r="H10" s="38"/>
-      <c r="I10" s="27" t="s">
+      <c r="G10" s="49"/>
+      <c r="H10" s="51"/>
+      <c r="I10" s="25" t="s">
         <v>16</v>
       </c>
     </row>
     <row r="11" spans="1:9" x14ac:dyDescent="0.45">
-      <c r="A11" s="44" t="s">
+      <c r="A11" s="41" t="s">
         <v>11</v>
       </c>
-      <c r="B11" s="11" t="s">
+      <c r="B11" s="8" t="s">
         <v>12</v>
       </c>
-      <c r="C11" s="11" t="s">
+      <c r="C11" s="8" t="s">
         <v>10</v>
       </c>
-      <c r="D11" s="21">
+      <c r="D11" s="19">
         <v>400</v>
       </c>
-      <c r="E11" s="11">
+      <c r="E11" s="8">
         <v>1832</v>
       </c>
-      <c r="F11" s="11">
+      <c r="F11" s="8">
         <v>1379</v>
       </c>
-      <c r="G11" s="5">
+      <c r="G11" s="2">
         <f>E11/$E$10</f>
         <v>3.982608695652174</v>
       </c>
-      <c r="H11" s="26">
+      <c r="H11" s="24">
         <f>F11/$F$10</f>
         <v>4.0204081632653059</v>
       </c>
-      <c r="I11" s="27" t="s">
+      <c r="I11" s="25" t="s">
         <v>20</v>
       </c>
     </row>
     <row r="12" spans="1:9" x14ac:dyDescent="0.45">
-      <c r="A12" s="44" t="s">
+      <c r="A12" s="41" t="s">
         <v>11</v>
       </c>
-      <c r="B12" s="11" t="s">
+      <c r="B12" s="8" t="s">
         <v>12</v>
       </c>
-      <c r="C12" s="11" t="s">
+      <c r="C12" s="8" t="s">
         <v>10</v>
       </c>
-      <c r="D12" s="21">
+      <c r="D12" s="19">
         <v>600</v>
       </c>
-      <c r="E12" s="11">
+      <c r="E12" s="8">
         <v>2748</v>
       </c>
-      <c r="F12" s="11">
+      <c r="F12" s="8">
         <v>2061</v>
       </c>
-      <c r="G12" s="5">
+      <c r="G12" s="2">
         <f t="shared" ref="G12:G13" si="2">E12/$E$10</f>
         <v>5.9739130434782606</v>
       </c>
-      <c r="H12" s="26">
+      <c r="H12" s="24">
         <f t="shared" ref="H12:H13" si="3">F12/$F$10</f>
         <v>6.0087463556851315</v>
       </c>
-      <c r="I12" s="27" t="s">
+      <c r="I12" s="25" t="s">
         <v>21</v>
       </c>
     </row>
     <row r="13" spans="1:9" x14ac:dyDescent="0.45">
-      <c r="A13" s="45" t="s">
+      <c r="A13" s="42" t="s">
         <v>11</v>
       </c>
-      <c r="B13" s="12" t="s">
+      <c r="B13" s="9" t="s">
         <v>12</v>
       </c>
-      <c r="C13" s="12" t="s">
+      <c r="C13" s="9" t="s">
         <v>10</v>
       </c>
-      <c r="D13" s="22">
+      <c r="D13" s="20">
         <v>800</v>
       </c>
-      <c r="E13" s="13">
+      <c r="E13" s="10">
         <v>3664</v>
       </c>
-      <c r="F13" s="13">
+      <c r="F13" s="10">
         <v>2743</v>
       </c>
-      <c r="G13" s="49">
+      <c r="G13" s="44">
         <f t="shared" si="2"/>
         <v>7.965217391304348</v>
       </c>
-      <c r="H13" s="52">
+      <c r="H13" s="47">
         <f t="shared" si="3"/>
         <v>7.9970845481049562</v>
       </c>
-      <c r="I13" s="28" t="s">
+      <c r="I13" s="26" t="s">
         <v>22</v>
       </c>
     </row>
     <row r="14" spans="1:9" x14ac:dyDescent="0.45">
-      <c r="A14" s="39" t="s">
+      <c r="A14" s="36" t="s">
         <v>25</v>
       </c>
-      <c r="B14" s="40" t="s">
+      <c r="B14" s="37" t="s">
         <v>12</v>
       </c>
-      <c r="C14" s="40" t="s">
+      <c r="C14" s="37" t="s">
         <v>13</v>
       </c>
-      <c r="D14" s="41">
+      <c r="D14" s="38">
         <v>50</v>
       </c>
-      <c r="E14" s="40">
+      <c r="E14" s="37">
         <v>378</v>
       </c>
-      <c r="F14" s="40">
+      <c r="F14" s="37">
         <v>167</v>
       </c>
-      <c r="G14" s="42">
+      <c r="G14" s="39">
         <f>E14/$E$15</f>
         <v>0.50132625994694957</v>
       </c>
-      <c r="H14" s="50">
+      <c r="H14" s="45">
         <f>F14/$F$15</f>
         <v>0.47308781869688388</v>
       </c>
-      <c r="I14" s="34" t="s">
+      <c r="I14" s="32" t="s">
         <v>28</v>
       </c>
     </row>
     <row r="15" spans="1:9" x14ac:dyDescent="0.45">
-      <c r="A15" s="43" t="s">
+      <c r="A15" s="40" t="s">
         <v>8</v>
       </c>
-      <c r="B15" s="18" t="s">
+      <c r="B15" s="16" t="s">
         <v>12</v>
       </c>
-      <c r="C15" s="18" t="s">
+      <c r="C15" s="16" t="s">
         <v>13</v>
       </c>
-      <c r="D15" s="21">
+      <c r="D15" s="16">
         <v>100</v>
       </c>
-      <c r="E15" s="18">
+      <c r="E15" s="16">
         <v>754</v>
       </c>
-      <c r="F15" s="18">
+      <c r="F15" s="16">
         <v>353</v>
       </c>
-      <c r="G15" s="16"/>
-      <c r="H15" s="17"/>
-      <c r="I15" s="34" t="s">
+      <c r="G15" s="14"/>
+      <c r="H15" s="15"/>
+      <c r="I15" s="32" t="s">
         <v>17</v>
       </c>
     </row>
     <row r="16" spans="1:9" x14ac:dyDescent="0.45">
-      <c r="A16" s="44" t="s">
+      <c r="A16" s="41" t="s">
         <v>11</v>
       </c>
-      <c r="B16" s="11" t="s">
+      <c r="B16" s="8" t="s">
         <v>12</v>
       </c>
-      <c r="C16" s="11" t="s">
+      <c r="C16" s="8" t="s">
         <v>13</v>
       </c>
-      <c r="D16" s="21">
+      <c r="D16" s="19">
         <v>400</v>
       </c>
-      <c r="E16" s="11">
+      <c r="E16" s="8">
         <v>3006</v>
       </c>
-      <c r="F16" s="11">
+      <c r="F16" s="8">
         <v>1419</v>
       </c>
-      <c r="G16" s="7">
+      <c r="G16" s="4">
         <f>E16/$E$15</f>
         <v>3.9867374005305041</v>
       </c>
-      <c r="H16" s="23">
+      <c r="H16" s="21">
         <f>F16/$F$15</f>
         <v>4.0198300283286121</v>
       </c>
-      <c r="I16" s="34" t="s">
+      <c r="I16" s="32" t="s">
         <v>18</v>
       </c>
     </row>
     <row r="17" spans="1:9" x14ac:dyDescent="0.45">
-      <c r="A17" s="44" t="s">
+      <c r="A17" s="41" t="s">
         <v>11</v>
       </c>
-      <c r="B17" s="11" t="s">
+      <c r="B17" s="8" t="s">
         <v>12</v>
       </c>
-      <c r="C17" s="11" t="s">
+      <c r="C17" s="8" t="s">
         <v>13</v>
       </c>
-      <c r="D17" s="21">
+      <c r="D17" s="19">
         <v>600</v>
       </c>
-      <c r="E17" s="11">
+      <c r="E17" s="8">
         <v>4510</v>
       </c>
-      <c r="F17" s="11">
+      <c r="F17" s="8">
         <v>2122</v>
       </c>
-      <c r="G17" s="7">
+      <c r="G17" s="4">
         <f t="shared" ref="G17:G18" si="4">E17/$E$15</f>
         <v>5.9814323607427058</v>
       </c>
-      <c r="H17" s="23">
+      <c r="H17" s="21">
         <f t="shared" ref="H17:H18" si="5">F17/$F$15</f>
         <v>6.0113314447592066</v>
       </c>
-      <c r="I17" s="34" t="s">
+      <c r="I17" s="32" t="s">
         <v>30</v>
       </c>
     </row>
     <row r="18" spans="1:9" ht="14.65" thickBot="1" x14ac:dyDescent="0.5">
-      <c r="A18" s="45" t="s">
+      <c r="A18" s="42" t="s">
         <v>11</v>
       </c>
-      <c r="B18" s="12" t="s">
+      <c r="B18" s="9" t="s">
         <v>12</v>
       </c>
-      <c r="C18" s="12" t="s">
+      <c r="C18" s="9" t="s">
         <v>13</v>
       </c>
-      <c r="D18" s="22">
+      <c r="D18" s="20">
         <v>800</v>
       </c>
-      <c r="E18" s="12">
+      <c r="E18" s="9">
         <v>6012</v>
       </c>
-      <c r="F18" s="12">
+      <c r="F18" s="9">
         <v>2824</v>
       </c>
-      <c r="G18" s="24">
+      <c r="G18" s="22">
         <f t="shared" si="4"/>
         <v>7.9734748010610081</v>
       </c>
-      <c r="H18" s="25">
+      <c r="H18" s="23">
         <f t="shared" si="5"/>
         <v>8</v>
       </c>
-      <c r="I18" s="36" t="s">
+      <c r="I18" s="34" t="s">
         <v>29</v>
       </c>
     </row>

</xml_diff>